<commit_message>
bugs/optimizaciones en inventarios, cierre mes y cardex
</commit_message>
<xml_diff>
--- a/public/application/files/jasper/templates/cierremes.xlsx
+++ b/public/application/files/jasper/templates/cierremes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-27020" yWindow="0" windowWidth="25500" windowHeight="14620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -191,7 +191,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -200,23 +200,31 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="33">
@@ -584,7 +592,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -593,90 +601,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="28">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:8" ht="28">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="8" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:8" ht="18">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="6"/>
+      <c r="D6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -692,7 +700,6 @@
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>